<commit_message>
Rename quiz sheets to numeric codes (e.g., 1.1)
</commit_message>
<xml_diff>
--- a/app/data/quizzes/LA.xlsx
+++ b/app/data/quizzes/LA.xlsx
@@ -7,10 +7,10 @@
     <workbookView windowWidth="20490" windowHeight="7620" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="1.1_Intro_to_Vectors" sheetId="1" r:id="rId1"/>
-    <sheet name="1.2_Vector_Addition" sheetId="2" r:id="rId2"/>
-    <sheet name="1.3_Dot_Product" sheetId="3" r:id="rId3"/>
-    <sheet name="1.4_Vectors_in_AI" sheetId="4" r:id="rId4"/>
+    <sheet name="1.1" sheetId="1" r:id="rId1"/>
+    <sheet name="1.2" sheetId="2" r:id="rId2"/>
+    <sheet name="1.3" sheetId="3" r:id="rId3"/>
+    <sheet name="1.4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -3166,7 +3166,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>